<commit_message>
Update Vanern sources and values
</commit_message>
<xml_diff>
--- a/Table1_SOS_Lake_Summary.xlsx
+++ b/Table1_SOS_Lake_Summary.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ian_GIS\gleon\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -370,9 +365,6 @@
     <t>27°37', 81°19'</t>
   </si>
   <si>
-    <t>KAIT CAN YOU TELL WHAT THIS IS? http://www.jstor.org.proxy-remote.galib.uga.edu/stable/pdf/4315187.pdf?acceptTC=true</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Yao, H., McConnell, C., Somers, K. M., Yan, N. D., Watmough, S., &amp; Scheider, W. (2011). Nearshore human interventions reverse patterns of decline in lake calcium budgets in central Ontario as demonstrated by mass‐balance analyses. </t>
     </r>
@@ -417,6 +409,9 @@
   </si>
   <si>
     <t>mesotrophic</t>
+  </si>
+  <si>
+    <t>Kvarnas, H (2001) Morphometry and hydrology of the four large lakes of Sweden. Ambio 30(8): 467-474; other sources see CommentsQuirks file for links.</t>
   </si>
 </sst>
 </file>
@@ -896,7 +891,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -907,7 +902,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +996,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="3"/>
@@ -1246,7 +1241,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I10" s="6">
         <v>4831.9225000000006</v>
@@ -1295,9 +1290,15 @@
       <c r="H11" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="I11" s="6">
+        <v>4680000</v>
+      </c>
+      <c r="J11">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K11">
+        <v>0.61470000000000002</v>
+      </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3">
         <v>4.47</v>
@@ -1353,7 +1354,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1399,7 +1400,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add changes to Langtjern
</commit_message>
<xml_diff>
--- a/Table1_SOS_Lake_Summary.xlsx
+++ b/Table1_SOS_Lake_Summary.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ian_GIS\gleon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17952" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Lake</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>DOC</t>
-  </si>
-  <si>
-    <t>don't have</t>
   </si>
   <si>
     <t>Watershed % Wetland</t>
@@ -330,9 +327,6 @@
     </r>
   </si>
   <si>
-    <t>http://www.niva.no/en/langtjern</t>
-  </si>
-  <si>
     <t>59°06’, -13°62’</t>
   </si>
   <si>
@@ -417,6 +411,9 @@
   </si>
   <si>
     <t>mesotrophic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.niva.no/en/langtjern</t>
   </si>
 </sst>
 </file>
@@ -906,67 +903,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="12" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="12" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="J2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>8</v>
@@ -978,12 +975,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" s="8">
         <v>36.4</v>
@@ -1001,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="3"/>
@@ -1017,12 +1014,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -1031,12 +1028,12 @@
       <c r="H4" s="23"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="8">
         <v>71.400000000000006</v>
@@ -1054,7 +1051,7 @@
         <v>3.1</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" s="6">
         <v>528.27563249500008</v>
@@ -1078,12 +1075,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="8">
         <v>22.7</v>
@@ -1099,7 +1096,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="6">
         <v>480</v>
@@ -1107,22 +1104,22 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1" t="s">
-        <v>11</v>
+      <c r="M6" s="3">
+        <v>1.4</v>
       </c>
       <c r="N6" s="4">
-        <v>10</v>
+        <v>5.3</v>
       </c>
       <c r="O6" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="8">
         <v>3990</v>
@@ -1140,7 +1137,7 @@
         <v>6.2</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" s="6">
         <v>60403.9087</v>
@@ -1164,12 +1161,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="8">
         <v>421</v>
@@ -1178,12 +1175,12 @@
       <c r="H8" s="23"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="8">
         <v>149</v>
@@ -1201,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I9" s="6">
         <v>6752.4100000000008</v>
@@ -1223,12 +1220,12 @@
       </c>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="8">
         <v>1610</v>
@@ -1246,7 +1243,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I10" s="6">
         <v>4831.9225000000006</v>
@@ -1270,12 +1267,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="8">
         <v>565000</v>
@@ -1293,7 +1290,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="3"/>
@@ -1309,12 +1306,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="14" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="13">
         <v>1557</v>
@@ -1323,88 +1320,88 @@
         <v>12</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="15">
         <v>32000</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="16"/>
     </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
table 1 update to include years of data we have
</commit_message>
<xml_diff>
--- a/Table1_SOS_Lake_Summary.xlsx
+++ b/Table1_SOS_Lake_Summary.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\SOS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17952" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Lake</t>
   </si>
@@ -282,7 +277,7 @@
     <t>Sources (what can't be gleaned from GIS)</t>
   </si>
   <si>
-    <t>60°37’, -9°73’</t>
+    <t>59°06’, -13°62’</t>
   </si>
   <si>
     <r>
@@ -295,12 +290,15 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>°41', 95°13'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>43</t>
+      <t>°11', 89°42'</t>
+    </r>
+  </si>
+  <si>
+    <t>68°63', 149°61'</t>
+  </si>
+  <si>
+    <r>
+      <t>45</t>
     </r>
     <r>
       <rPr>
@@ -309,54 +307,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>°36', 95°15'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>43</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>°44', 95°34'</t>
-    </r>
-  </si>
-  <si>
-    <t>59°06’, -13°62’</t>
-  </si>
-  <si>
-    <r>
-      <t>43</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>°11', 89°42'</t>
-    </r>
-  </si>
-  <si>
-    <t>68°63', 149°61'</t>
-  </si>
-  <si>
-    <r>
-      <t>45</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>°38', 79°14'</t>
     </r>
   </si>
@@ -414,13 +364,34 @@
   </si>
   <si>
     <t xml:space="preserve"> http://www.niva.no/en/langtjern</t>
+  </si>
+  <si>
+    <t>Data years</t>
+  </si>
+  <si>
+    <t>2004-2013</t>
+  </si>
+  <si>
+    <t>2001-2013</t>
+  </si>
+  <si>
+    <t>2006-2013</t>
+  </si>
+  <si>
+    <t>1991-2001</t>
+  </si>
+  <si>
+    <t>Mar 08-May 10</t>
+  </si>
+  <si>
+    <t>2005-2008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -593,34 +564,39 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,7 +657,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -716,7 +692,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -893,514 +869,456 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="12" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" s="12" customFormat="1" ht="16.5" thickBot="1">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75">
       <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="B3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="8">
         <v>36.4</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>2760000</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>2334.768</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>10</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>2</v>
       </c>
-      <c r="H3" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="3"/>
+      <c r="I3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="6"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="3">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3">
         <v>2</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>5</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:16" ht="15.75">
+      <c r="A4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="8">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9500000</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="6">
+        <v>528.27563249500008</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="O4" s="3">
+        <v>5</v>
+      </c>
+      <c r="P4" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75">
+      <c r="A5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3990</v>
+      </c>
+      <c r="E5" s="2">
+        <v>505000000</v>
+      </c>
+      <c r="F5" s="3">
+        <v>35200</v>
+      </c>
+      <c r="G5" s="3">
+        <v>12.7</v>
+      </c>
+      <c r="H5" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="6">
+        <v>60403.9087</v>
+      </c>
+      <c r="K5" s="3">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="L5" s="3">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.626</v>
+      </c>
+      <c r="N5" s="3">
+        <v>2.84</v>
+      </c>
+      <c r="O5" s="4">
+        <v>20</v>
+      </c>
+      <c r="P5" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75">
+      <c r="A6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="8">
+        <v>149</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10600000</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8104</v>
+      </c>
+      <c r="G6" s="3">
+        <v>7</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="6">
+        <v>6752.4100000000008</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="O6" s="3">
+        <v>2</v>
+      </c>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75">
+      <c r="A7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1610</v>
+      </c>
+      <c r="E7" s="2">
+        <v>235000000</v>
+      </c>
+      <c r="F7" s="3">
+        <v>25900</v>
+      </c>
+      <c r="G7" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="6">
+        <v>4831.9225000000006</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.106</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="M7" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="N7" s="3">
+        <v>5.32</v>
+      </c>
+      <c r="O7" s="3">
+        <v>11</v>
+      </c>
+      <c r="P7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="14" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="13">
+        <v>565000</v>
+      </c>
+      <c r="E8" s="25">
+        <v>153000000000</v>
+      </c>
+      <c r="F8" s="26">
+        <v>2007000</v>
+      </c>
+      <c r="G8" s="26">
+        <v>27</v>
+      </c>
+      <c r="H8" s="26">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26">
+        <v>4.47</v>
+      </c>
+      <c r="O8" s="28">
+        <v>6.3</v>
+      </c>
+      <c r="P8" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75">
+      <c r="A11" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75">
+      <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="8">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="D5" s="2">
-        <v>9500000</v>
-      </c>
-      <c r="E5" s="3">
-        <v>4000</v>
-      </c>
-      <c r="F5" s="3">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="6">
-        <v>528.27563249500008</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="N5" s="3">
-        <v>5</v>
-      </c>
-      <c r="O5" s="3">
+      <c r="B14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75">
+      <c r="A15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75">
+      <c r="A16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75">
+      <c r="A17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75">
+      <c r="A19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75">
+      <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="8">
-        <v>22.7</v>
-      </c>
-      <c r="D6" s="1">
-        <v>454000</v>
-      </c>
-      <c r="E6" s="1">
-        <v>32448</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="6">
-        <v>480</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="N6" s="4">
-        <v>5.3</v>
-      </c>
-      <c r="O6" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="21" t="s">
+      <c r="B20" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="8">
-        <v>3990</v>
-      </c>
-      <c r="D7" s="2">
-        <v>505000000</v>
-      </c>
-      <c r="E7" s="3">
-        <v>35200</v>
-      </c>
-      <c r="F7" s="3">
-        <v>12.7</v>
-      </c>
-      <c r="G7" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="6">
-        <v>60403.9087</v>
-      </c>
-      <c r="J7" s="3">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="K7" s="3">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0.626</v>
-      </c>
-      <c r="M7" s="3">
-        <v>2.84</v>
-      </c>
-      <c r="N7" s="4">
-        <v>20</v>
-      </c>
-      <c r="O7" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="8">
-        <v>421</v>
-      </c>
-      <c r="G8"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="8">
-        <v>149</v>
-      </c>
-      <c r="D9" s="2">
-        <v>10600000</v>
-      </c>
-      <c r="E9" s="3">
-        <v>8104</v>
-      </c>
-      <c r="F9" s="3">
-        <v>7</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="6">
-        <v>6752.4100000000008</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.504</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>4.75</v>
-      </c>
-      <c r="N9" s="3">
-        <v>2</v>
-      </c>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1610</v>
-      </c>
-      <c r="D10" s="2">
-        <v>235000000</v>
-      </c>
-      <c r="E10" s="3">
-        <v>25900</v>
-      </c>
-      <c r="F10" s="3">
-        <v>14.6</v>
-      </c>
-      <c r="G10" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="6">
-        <v>4831.9225000000006</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0.106</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="L10" s="3">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="M10" s="3">
-        <v>5.32</v>
-      </c>
-      <c r="N10" s="3">
-        <v>11</v>
-      </c>
-      <c r="O10" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="8">
-        <v>565000</v>
-      </c>
-      <c r="D11" s="2">
-        <v>153000000000</v>
-      </c>
-      <c r="E11" s="3">
-        <v>2007000</v>
-      </c>
-      <c r="F11" s="3">
-        <v>27</v>
-      </c>
-      <c r="G11" s="3">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3">
-        <v>4.47</v>
-      </c>
-      <c r="N11" s="4">
-        <v>6.3</v>
-      </c>
-      <c r="O11" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="14" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="13">
-        <v>1557</v>
-      </c>
-      <c r="F12" s="14">
-        <v>12</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="15">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="16"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C20" s="22"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75">
       <c r="A21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
table 1 for paper
</commit_message>
<xml_diff>
--- a/Table1_SOS_Lake_Summary.xlsx
+++ b/Table1_SOS_Lake_Summary.xlsx
@@ -525,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -544,18 +544,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -869,7 +863,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -880,14 +874,14 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="3" width="13.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -904,73 +898,73 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="12" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:16" s="11" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>36.4</v>
       </c>
       <c r="E3" s="2">
         <v>2760000</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
         <v>2334.768</v>
       </c>
       <c r="G3" s="3">
@@ -979,7 +973,7 @@
       <c r="H3" s="3">
         <v>2</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="18" t="s">
         <v>41</v>
       </c>
       <c r="J3" s="6"/>
@@ -997,22 +991,22 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>71.400000000000006</v>
       </c>
       <c r="E4" s="2">
         <v>9500000</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>4000</v>
       </c>
       <c r="G4" s="3">
@@ -1021,7 +1015,7 @@
       <c r="H4" s="3">
         <v>3.1</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="18" t="s">
         <v>26</v>
       </c>
       <c r="J4" s="6">
@@ -1047,31 +1041,31 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>3990</v>
       </c>
       <c r="E5" s="2">
         <v>505000000</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>35200</v>
       </c>
       <c r="G5" s="3">
-        <v>12.7</v>
+        <v>13</v>
       </c>
       <c r="H5" s="3">
         <v>6.2</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="18" t="s">
         <v>25</v>
       </c>
       <c r="J5" s="6">
@@ -1097,22 +1091,22 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>149</v>
       </c>
       <c r="E6" s="2">
         <v>10600000</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>8104</v>
       </c>
       <c r="G6" s="3">
@@ -1121,7 +1115,7 @@
       <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="18" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="6">
@@ -1145,31 +1139,31 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="15.75">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>1610</v>
       </c>
       <c r="E7" s="2">
         <v>235000000</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>25900</v>
       </c>
       <c r="G7" s="3">
-        <v>14.6</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="18" t="s">
         <v>26</v>
       </c>
       <c r="J7" s="6">
@@ -1194,50 +1188,50 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="14" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:16" s="12" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="13">
         <v>565000</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="23">
         <v>153000000000</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="13">
         <v>2007000</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="24">
         <v>27</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="24">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26">
+      <c r="J8" s="13"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24">
         <v>4.47</v>
       </c>
-      <c r="O8" s="28">
+      <c r="O8" s="26">
         <v>6.3</v>
       </c>
-      <c r="P8" s="28">
+      <c r="P8" s="26">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="21" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1245,26 +1239,26 @@
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:16" ht="15.75">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
     </row>
     <row r="14" spans="1:16" ht="15.75">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="14"/>
     </row>
     <row r="15" spans="1:16" ht="15.75">
       <c r="A15" s="5" t="s">
@@ -1294,28 +1288,28 @@
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" ht="15.75">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="20"/>
     </row>
     <row r="21" spans="1:3" ht="15.75">
       <c r="A21" s="5" t="s">

</xml_diff>

<commit_message>
updated citation for Vanern data source
</commit_message>
<xml_diff>
--- a/Table1_SOS_Lake_Summary.xlsx
+++ b/Table1_SOS_Lake_Summary.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ian_GIS\gleon\SOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kfarrell\Documents\R\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
@@ -240,9 +240,6 @@
     <t>27°37', 81°19'</t>
   </si>
   <si>
-    <t>KAIT CAN YOU TELL WHAT THIS IS? http://www.jstor.org.proxy-remote.galib.uga.edu/stable/pdf/4315187.pdf?acceptTC=true</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Yao, H., McConnell, C., Somers, K. M., Yan, N. D., Watmough, S., &amp; Scheider, W. (2011). Nearshore human interventions reverse patterns of decline in lake calcium budgets in central Ontario as demonstrated by mass‐balance analyses. </t>
     </r>
@@ -484,11 +481,14 @@
   <si>
     <t>Table 2. Lake model parameters</t>
   </si>
+  <si>
+    <t>Kvarnäs, H. 2001. Morphometry and Hydrology of the Four Large Lakes of Sweden. Ambio 30: 467-474</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,19 +1039,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>16</v>
@@ -1066,13 +1066,13 @@
         <v>20</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N2" s="20" t="s">
         <v>19</v>
@@ -1093,13 +1093,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="25">
         <v>36.4</v>
@@ -1117,7 +1117,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="27">
         <v>2</v>
@@ -1139,13 +1139,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="25">
         <v>71.400000000000006</v>
@@ -1193,13 +1193,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="25">
         <v>3990</v>
@@ -1247,13 +1247,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="25">
         <v>149</v>
@@ -1301,13 +1301,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="25">
         <v>1610</v>
@@ -1355,13 +1355,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="32">
         <v>565000</v>
@@ -1422,7 +1422,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -1431,7 +1431,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="5"/>
     </row>
@@ -1480,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C21" s="6"/>
     </row>
@@ -1499,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,12 +1512,12 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>6</v>
@@ -1540,7 +1540,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="10">
         <v>364000</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="10">
         <v>2760000</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>3.992</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0.54</v>
@@ -1689,12 +1689,12 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11">
         <v>0.01</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="11">
         <v>27</v>
@@ -1740,12 +1740,12 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>0.29099999999999998</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.41099999999999998</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18">
@@ -1858,7 +1858,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19">
@@ -1877,7 +1877,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>0.9</v>
@@ -1900,7 +1900,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1923,12 +1923,12 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23">
         <v>0.01</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="11">
         <v>1E-3</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="38">
         <v>0.8</v>

</xml_diff>

<commit_message>
Filling in parameter descriptions
</commit_message>
<xml_diff>
--- a/Table1_SOS_Lake_Summary.xlsx
+++ b/Table1_SOS_Lake_Summary.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="139">
   <si>
     <t>Lake</t>
   </si>
@@ -582,10 +582,28 @@
     <t>Proportion of catchment with tree cover</t>
   </si>
   <si>
-    <t>Proportion of catchment wetlands</t>
-  </si>
-  <si>
     <t>Proportion of lake inflow as groundwater</t>
+  </si>
+  <si>
+    <t>Loading rate of POC from wetlands</t>
+  </si>
+  <si>
+    <t>Proportion of catchment that is wetlands</t>
+  </si>
+  <si>
+    <t>Lake water DOC concentration at start of model run</t>
+  </si>
+  <si>
+    <t>Lake water POC concentration at start of model run</t>
+  </si>
+  <si>
+    <t>DOC concentration of groundwater</t>
+  </si>
+  <si>
+    <t>DOC concentration of precipitation</t>
+  </si>
+  <si>
+    <t>Influx of aerial POC (e.g., leaf litter)</t>
   </si>
 </sst>
 </file>
@@ -844,7 +862,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -879,7 +897,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1510,7 +1528,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1659,6 +1677,9 @@
       <c r="A8" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="C8" s="3">
         <v>3.7</v>
       </c>
@@ -1679,6 +1700,9 @@
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="C9" s="3">
         <v>0.37</v>
       </c>
@@ -1797,7 +1821,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -1819,6 +1843,9 @@
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="C17" s="3">
         <v>1</v>
       </c>
@@ -1839,6 +1866,9 @@
       <c r="A18" s="3" t="s">
         <v>125</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="C18" s="3">
         <v>10</v>
       </c>
@@ -1860,7 +1890,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -1882,6 +1912,9 @@
       <c r="A20" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="B20" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="C20" s="3">
         <v>2</v>
       </c>
@@ -1976,6 +2009,9 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>

</xml_diff>